<commit_message>
Flask and live application!!
</commit_message>
<xml_diff>
--- a/openai/algabo_results.xlsx
+++ b/openai/algabo_results.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Algabo - Quitamanchas con dosificador - 120 ml</t>
+          <t>Algabo - Quitamanchas con Dosificador - 120 ml</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Algabo Kids - Shampoo Sandía - 350 ml</t>
+          <t>Algabo Kids - Shampoo Sandía Sweet - 350 ml</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Algabo - Quita Manchas Negras - 100 ml</t>
+          <t>Algabo - Removedor de Manchas Negras - 100 ml</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Algabo - Quita Manchas Xtreme - Profesional - 100 ml</t>
+          <t>Algabo - Removedor de Manchas Xtreme - 100 ml</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Algabo - Quita Keratina - 100 ml</t>
+          <t>Algabo - Removedor de Queratina - 100 ml</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Algabo - Quita Fortalecedor - 100 ml</t>
+          <t>Algabo - Quitaesmalte Fortalecedor - 100 ml</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Algabo - Quita Manchas Express - 75 ml</t>
+          <t>Algabo - Quita Manchas Express - 75 ml - Sin Esfuerzo</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Algabo - Gel Sanitizante Ultra - Eco Pack - 1000 ml</t>
+          <t>Algabo - Gel Sanitizante Ultra - 1000 ml - Transparente - Fórmula de Secado Rápido</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Algabo - Quita Cutículas con Keratina - 50 ml</t>
+          <t>Algabo - Quitaesmalte con Keratina - 50 ml</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Algabo - Quita Humectante - 50 ml</t>
+          <t>Algabo - Quita Humectante - 50 ml - Sin residuos</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Algabo - Quita Fortalecedor - 50 ml</t>
+          <t>Algabo - Quita Esmalte Fortalecedor - 50 ml</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido El 10 - Botella 300 ml</t>
+          <t>Algabo - Jabón Líquido - 300 ml - Transparente</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Algabo - Gel Sanitizante Fresh - 250 ml</t>
+          <t>Algabo - Gel Sanitizante Fresco - 250 ml</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Algabo Kids - Shampoo Melocotón - 350 ml</t>
+          <t>Algabo Kids - Shampoo Melocotón - 350 ml - Fragancia suave y nutritiva</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Algabo Kids - Shampoo Chicle - 350 ml</t>
+          <t>Algabo Kids - Shampoo Bubble Gum - 350 ml - Rosa - Sin lágrimas</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo Coco y Leche - Envase Pequeño - 300 ml</t>
+          <t>Algabo - Shampoo Coco y Leche - 300 ml - Eco Pack</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo Manzanilla y Magnolia - Eco Pack - 300 ml</t>
+          <t>Algabo - Shampoo Manzana y Magnolia - Eco Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo Detox - Eco Pack - 300 ml</t>
+          <t>Algabo - Shampoo Detox - 300 ml</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Algabo Kids - Shampoo Sandía - 750 ml</t>
+          <t>Algabo Kids - Shampoo Sandía Dulce - 750 ml</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Chapoteando - Shampoo Trolls Branch - 750 ml</t>
+          <t>Chapoteando - Shampoo Trolls Branch - 750 ml - Azul - Fórmula suave</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Trolls - Shampoo Poppi - 750 ml - Cabello brillante</t>
+          <t>Trolls - Shampoo Poppi - 750 ml - Rosa - Delicadamente perfumado</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo Aguacate y Argán - 930 ml</t>
+          <t>Algabo - Shampoo Nutritivo - 930 ml - Aguacate y Argán</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo Manzana y Magnolia - 930 ml</t>
+          <t>Algabo - Shampoo de Manzana y Magnolia - 930 ml</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo 0% Açaí y Romero - 750 ml</t>
+          <t>Algabo - Shampoo 0% Sal - Sin Sal - Acai y Romero - 750 ml</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Algabo Kids - Acondicionador Sandía Dulce - 350 ml</t>
+          <t>Algabo Kids - Sandía Sweet Bath Gel - 350 ml</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Floral - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Floral - Doy Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Flower Mix - 300 ml</t>
+          <t>Algabo - Jabón Líquido Floral - 300 ml - Mezcla de Flores</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Coco - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido de Coco - 300 ml</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Bosque - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Bosque - Doy Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Coco - 300 ml</t>
+          <t>Algabo - Jabón Líquido de Coco - 300 ml</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Bosque - 300 ml</t>
+          <t>Algabo - Jabón Líquido Frescura Bosque - 300 ml</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Té Verde - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Verde - Doy Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Citrus - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Cítrico - 300 ml - Citrus Fresh</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Floral Rain - 300 ml</t>
+          <t>Algabo - Jabón Líquido Floral Rain - 300 ml - Transparente &amp; Refrescante</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido de Citrus - 300 ml</t>
+          <t>Algabo - Jabón Líquido Cítrico - 300 ml</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Algabo - Alcohol en Aerosol - 140 ml</t>
+          <t>Algabo - Alcohol en Aerosol Ultra - 140 ml</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Cremoso - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Cremoso - 300 ml</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Floral - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Floral - 300 ml - Suave y Perfumado</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Algabo - Espuma Manzanilla Mágica - Doypack - 250 ml</t>
+          <t>Algabo - Jabón Espumoso Manzana y Magnolia - 250 ml - Doy Pack</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Coco y Miel - Doypack 220 ml</t>
+          <t>Algabo - Jabón Líquido Cocomiel - 220 ml</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Karité y Aguacate - Doypack - 220 ml</t>
+          <t>Algabo - Jabón Líquido Kar-Agu - 220 ml - Transparente - Con aroma a karité y aguacate</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Algabo - Spray Sanitizante Ultra - 500 ml</t>
+          <t>Algabo - Spray Sanitario Ultra - 500 ml</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Algabo - Sanitizante Manos - 4 oz - Glicerina</t>
+          <t>Algabo - Gel Sanitizante Ultra - 4 oz - Sin Glicerina - Para Manos</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Algabo - Sanitizante Superficies - 4 unidades</t>
+          <t>Algabo - Limpiador Superficies Ultra Sanitizante - 4 Unidades</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Algabo - Gel Sanitizante Manos - 4 oz - Con Glicerina</t>
+          <t>Algabo - Gel Sanitario Glicerina - 4 unidades - Transparente - Cuidado de manos</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Citrus - Eco Pack - 900 ml</t>
+          <t>Algabo - Jabón Líquido Cítrico - 900 ml</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Té Verde - Eco Pack - 900 ml</t>
+          <t>Algabo - Jabón líquido - Té verde - 900 ml</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Floral - Eco Pack - 900 ml</t>
+          <t>Algabo - Jabón Líquido Floral - 900 ml</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Antibacterial - Eco Pack - 900 ml</t>
+          <t>Algabo - Jabón Líquido Antibacterial - 900 ml</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Karité y Aguacate - 221 ml</t>
+          <t>Algabo - Jabón Líquido Karité-Agua - 221 ml</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Algabo - Shampoo 0% Oliva y Argán - 750 ml</t>
+          <t>Algabo - Champú 0% Sal - Sin Sal - Oliva y Argan - 750 ml</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador Aguacate y Argán - Eco Pack - 300 ml</t>
+          <t>Algabo - Acondicionador Nutritivo Aguacate y Argán - Eco Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Algabo - Sanitizante Doypack - 300 ml</t>
+          <t>Algabo - Sanitizante de Superficie - 300 ml - Sin Enjuague</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Algabo - Gel Silver Gota - 150 ml</t>
+          <t>Algabo - Gel Plateado - 150 ml</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Algabo - Gel de Brillo Extra - Pomo 150 ml</t>
+          <t>Algabo - Gel Capilar Brillo - 150 ml</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Algabo - Gel Húmedo - Pomo 150 ml</t>
+          <t>Algabo - Gel Hidratante - 150 ml - Efecto Húmedo</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Fuerte - Pomo 200 ml</t>
+          <t>Algabo - Gel Extra Fuerte - 200 ml - Transparente - Fijación duradera</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Brillo - Pomo 200 ml</t>
+          <t>Algabo - Gel Brillo - 200 ml - Transparente - Aporta brillo duradero</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Algabo - Gel Efecto Húmedo - Pomo 200 ml</t>
+          <t>Algabo - Gel Hidratante - 200 ml - Sin Enjuague - Efecto Húmedo</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Algabo - Gel Titanium - 150 ml</t>
+          <t>Algabo - Gel Capilar Titanium - 150 ml</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Algabo - Gel Chrome - 150 gotas - Plateado</t>
+          <t>Algabo - Gel Capilar Gota Chrome - 150 ml</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Algabo - Hisopos Tubo - 200 unidades</t>
+          <t>Algabo - Hisopos de Algodón - 200 unidades - Blanco - Suaves y absorbentes</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Algabo - Baño Natural - Pomo 200 ml</t>
+          <t>Algabo - Baño Natural - 200 ml - Sin químicos - Pomo</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Algabo - Baño Natural Argán - 350 ml</t>
+          <t>Algabo - Gel de Baño Argan - 350 ml - Natural y Suave</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Algabo - Barro Vegetal - Pomo - 200 ml</t>
+          <t>Algabo - Mascarilla de Barro Vegetal - 200g</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Algabo - Mascarilla de Barro Vegetal - Pote 350 ml</t>
+          <t>Algabo - Mascarilla de Barro Vegetal - 350g - Pote - Purificante y Nutritiva</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Algabo - Crema Peinar Argán - 300 ml</t>
+          <t>Algabo - Crema de Peinar - Argán - 300 ml</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Algabo - Crema para Peinar Keratina - 300 ml</t>
+          <t>Algabo - Crema de Peinar Kerat - 300 ml - Sin Enjuague - Protección y Nutrición</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Fuerte - Pomo 150 ml</t>
+          <t>Algabo - Gel Extra Fuerte - 150 ml - Transparente - Fijación duradera</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Algabo - Gel Refrescante - 475 ml - Hidratante - Efecto Húmedo</t>
+          <t>Algabo - Gel Hidratante - 475 ml - Sin Enjuague - Fórmula Humectante</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Brillo - 475 ml</t>
+          <t>Algabo - Gel Capilar Brillo Extremo - 475 ml</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Fuerte - 475 ml</t>
+          <t>Algabo - Gel Capilar Extra Fuerte - 475 ml</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Algabo - Gel Higienizante Húmedo - Pote 350 ml</t>
+          <t>Algabo - Gel Hidratante - Pote 350 - Efecto Húmedo</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Algabo - Gel Brillo Intenso - Pote 350 ml</t>
+          <t>Algabo - Gel Capilar Extra Brillo - 350 ml</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Algabo - Gel Extra Fuerte - Pote 350 ml</t>
+          <t>Algabo - Gel Capilar Extra Fuerte - Pote 350 ml</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Algabo - Gel Chrome - 500 ml</t>
+          <t>Algabo - Gel Capilar Chrome - 500 ml</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Algabo - Gel Silver - 500 ml</t>
+          <t>Algabo - Gel Capilar Silver - 500 ml</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Algabo - Gel Titanium - 500 ml</t>
+          <t>Algabo - Gel Capilar Premium Titanium - 500 ml</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Algabo - Talco Men - 120 g</t>
+          <t>Algabo - Talco para Hombres - 120 gr</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Algabo - Talco para hombres - 180 g</t>
+          <t>Algabo - Talco para hombres - 180 gr</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Algabo - After Shave Men - 120 ml</t>
+          <t>Algabo - After Shave para Hombres - 120 ml</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Algabo - Crema de Afeitar Men - 150 ml</t>
+          <t>Algabo - Crema de Afeitar para Hombres - 150 ml</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Algabo - Espuma de Afeitar Men - 415 ml</t>
+          <t>Algabo - Espuma de Afeitar para Hombres - 415 ml</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Algabo - Espuma de Afeitar Men - 200 ml</t>
+          <t>Algabo - Espuma de Afeitar para Hombres - 200 ml</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Algabo - Crema de Afeitar - Pomo 177 ml</t>
+          <t>Algabo - Crema de Afeitar para Hombres - 177 ml</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Algabo - Hisopos Tubo - 125 unidades</t>
+          <t>Algabo - Hisopos de Algodón en Tubo - 125 unidades</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador Aguacate y Argán - Eco Pack - 930 ml</t>
+          <t>Algabo - Acondicionador Aguacate y Argán - 930 ml</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Algabo - Crema Suavizante Avena-Karité - 400 ml</t>
+          <t>Algabo - Crema Avena-Karité - 400 ml - Nutritiva - Piel suave y sedosa</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Algabo - Crema Aloe Manzanilla - 400 ml</t>
+          <t>Algabo - Crema Aloe y Manzanilla - 400 ml</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador 0% Oliva y Argán - 750 ml</t>
+          <t>Algabo - Acondicionador Sin Sal - Oliva y Argán - 750 ml</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador sin Aclarado - 0% Açaí y Romero - 750 ml</t>
+          <t>Algabo - Acondicionador Sin Sal - Açaí y Romero - 750 ml</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador Manzanilla y Magnolia - Eco Pack - 930 ml</t>
+          <t>Algabo - Perfume de Manzana y Magnolia - 930ml</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador Manzana y Magnolia - 930 ml</t>
+          <t>Algabo - Acondicionador de Manzana y Magnolia - 930 ml</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Algabo - Hisopos Tubo - 125 unidades</t>
+          <t>Algabo - Hisopos de Algodón en Tubo - 125 unidades</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Algabo - Acondicionador Aguacate y Argán - 930 ml</t>
+          <t>Algabo - Acondicionador Aguacate y Argan - 930 ml</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Trolls - Acondicionador Poppi - 750 ml</t>
+          <t>Trolls - Acondicionador Poppi - 750 ml - Rosa brillante - Suavidad y brillo intenso</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Algabo - Mascarilla Facial Detox - Eco Pack - 300 ml</t>
+          <t>Algabo - Acondicionador Detox - 300 ml - Frescura Natural</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Algabo - Crema Miel-Almendra - 400 ml</t>
+          <t>Algabo - Crema Miel-Almendra - 400 ml - Suavidad y Nutrición</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Algabo - Crema Manos y Uñas - 90 ml</t>
+          <t>Algabo - Crema Manos y Uñas - 90 ml - Hidratante - Fortalece las uñas</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Algabo - Crema Nutritiva Avena y Karité - 200 ml</t>
+          <t>Algabo - Crema Avena-Karité - 200 ml - Hidratación intensa</t>
         </is>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Algabo - Crema Aloe y Manzanilla - 200 ml</t>
+          <t>Algabo - Crema Aloe-Manzanilla - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Algabo - Agua Micelar - Dosificador - 120 ml</t>
+          <t>Algabo - Agua Micelar Suave - 120 ml</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Algabo - Agua Micelar Suave - 200 ml</t>
+          <t>Algabo - Agua Micelar - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Algabo - Enjuague Bucal Frescura 500 - 500 ml</t>
+          <t>Algabo - Enjuague Bucal Refrescante - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Algabo - Enjuague Bucal Fresh - 250 ml</t>
+          <t>Algabo - Enjuague Bucal Refrescante - 250 ml</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Algabo - Enjuague Bucal sin Alcohol - 250 ml</t>
+          <t>Algabo - Enjuague Bucal Sin Alcohol - 250 ml</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Algabo - Hisopos de Algodón - Tubo - 100 unidades</t>
+          <t>Algabo - Hisopos de Algodón en Tubo - 100 unidades</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Algabo - Hisopos Zipper - 125 unidades</t>
+          <t>Algabo - Hisopos Zipper - 125 unidades - Blanco - Cierre fácil y seguro</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Algabo - Porta Gel Sanitizante - 30 ml</t>
+          <t>Algabo - Soporte para Gel Sanitizante - 30 ml</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Algabo Baby - Jabón Pastilla Suave - 80 g</t>
+          <t>Algabo Baby - Jabón Suave - 80 g</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Algabo Baby - Shampoo Manzanilla - 200 ml</t>
+          <t>Algabo Baby - Shampoo Manzanilla Suave - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Algabo Kids - Shampoo Anti Piojos Zero - 500 ml</t>
+          <t>Algabo Kids - Shampoo Anti-Piojos - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Algabo Baby - Shampoo Suave 200 ml</t>
+          <t>Algabo Baby - Shampoo Suavidad Pura - 200 ml - Transparente - Sin lágrimas</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Algabo Baby - Jabón Líquido Suave - 200 ml</t>
+          <t>Algabo Baby - Jabón Líquido Suave - 200 ml - Sin Lágrimas</t>
         </is>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Algabo Baby - Jabón Líquido con Válvula - 200 ml</t>
+          <t>Algabo Baby - Jabón Líquido Suave - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Algabo Baby - Jabón Pastilla - Pack 80 unidades</t>
+          <t>Algabo Baby - Jabón Suave - 80g - Blanco - Fórmula delicada para bebés</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Algabo Kids - Loción Zero - 100 ml</t>
+          <t>Algabo Kids - Loción Zero - 100 ml - Sin fragancia - Hidratación suave</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Ultra Zombies - Jabón Líquido - Botella de 300 ml</t>
+          <t>Ultra Zombies - Jabón Líquido - 300 ml - Transparente - Fórmula suave y refrescante</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Algabo Baby - Colonia Dulces Mimos - 125 ml</t>
+          <t>Algabo Baby - Colonia Dulces Mimos - 125 ml - Fragancia suave</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Algabo Baby - Colonia Brisa Suave - 200 ml</t>
+          <t>Algabo Baby - Colonia Fresca - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Algabo Baby - Colonia Mimos - 200 ml</t>
+          <t>Algabo Baby - Colonia Dulces Mimos - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Algabo Baby - Fécula Doypack - 200 g</t>
+          <t>Algabo Baby - Fécula en Bolsa - 200 g</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Algabo Baby - Talquera de Fécula - 200 g</t>
+          <t>Algabo Baby - Talquera de Fécula - 200 g - Blanco - Suave y absorbente</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Algabo Baby - Set Colonia y Shampoo - 125 ml + 200 ml</t>
+          <t>Algabo Baby - Set Dulces Mimos - 125 ml Colonia + 200 ml Shampoo</t>
         </is>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Algabo Baby - Shampoo Suavidad Total - 444 ml</t>
+          <t>Algabo Baby - Shampoo de Bebé Suave - 444 ml</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Algabo Baby - Shampoo Manzanilla Suave - 444 ml</t>
+          <t>Algabo Baby - Shampoo Suave - 444 ml - Manzanilla - Sin lágrimas</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Algabo Baby - Shampoo Manzanilla - 755 ml</t>
+          <t>Algabo Baby - Shampoo Suave - 755 ml</t>
         </is>
       </c>
     </row>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Algabo Kids - Spray Antipiojos Zero - 500 ml</t>
+          <t>Algabo Kids - Aco Piojos - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Algabo Baby - Acondicionador Extra Suave - 444 ml</t>
+          <t>Algabo Baby - Acondicionador Suave - 444 ml</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Algabo Baby - Toallitas Húmedas - 20 unidades</t>
+          <t>Algabo Baby - Toallitas Húmedas - 20 unidades - Suave y delicado</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Algabo Baby - Toallitas Húmedas - 48 unidades</t>
+          <t>Algabo Baby - Toallitas Húmedas - 48 unidades - Sin fragancia - Ultra suaves</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Algabo Baby - Toallitas Húmedas - 80 unidades</t>
+          <t>Algabo Baby - Toallas Húmedas - 80 unidades</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Algabo Baby - Toallitas Húmedas - 100 unidades</t>
+          <t>Algabo Baby - Toallas Húmedas Suaves - 100 unidades</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Algabo Baby - Toallas Húmedas 3x48 - 15% Descuento</t>
+          <t>Algabo Baby - Toallas Húmedas - Pack de 3 - 48 unidades - 15% de descuento</t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Algabo Baby - Oleo Calcáreo - 500 ml</t>
+          <t>Algabo Baby - Aceite Calcáreo - 500 ml - Sin fragancia - Para cuidado infantil</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Algabo Baby - Aceite de Calcáreo - 500 ml</t>
+          <t>Algabo Baby - Oleo Calcáreo Suave - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Algabo Baby - Oleo Calcareo - Eco Pack - 900 ml</t>
+          <t>Algabo Baby - Oleo Calcáreo Spray - 900 ml - Transparente - Fácil aplicación</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Algabo Baby - Hisopos de Algodón - Caja 30 unidades</t>
+          <t>Algabo Baby - Caja de hisopos de algodón - 30 unidades - Blanco puro</t>
         </is>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Ultra Zombies - Autito 2 en 1 - 450 ml</t>
+          <t>Ultra Zombies - Shampoo + Gel de Ducha - 2 en 1 - Forma de autito - 450 ml</t>
         </is>
       </c>
     </row>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Algabo - Set Hello Kitty - 125 ml + 200 ml</t>
+          <t>Algabo - Set Hello Kitty - Colonia 125 ml + Shampoo 200 ml - Rosa - Cabello suave y fragante</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Vais - Detergente Lavavajillas - Eco Pack - 800 ml</t>
+          <t>Vais - Lavavajillas - 800 ml - Sin esfuerzo</t>
         </is>
       </c>
     </row>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Vais - Algodón Suave - 4 unidades</t>
+          <t>Vais - Pompones de Algodón - Pack de 4</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Fresco Primavera - 4 unidades</t>
+          <t>Vais - Limpiador Fresco - Primavera - 4 Litros</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Cítrico - 900 ml</t>
+          <t>Vais - Limpiador Cítrico - 900 ml - Frescura Cítrica</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Lavanda - 900 ml</t>
+          <t>Vais - Limpiador de Lavanda - 900 ml - Aroma Relajante</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Vais - Pompones de Algodón - 900 unidades</t>
+          <t>Vais - Pompones de Algodón - 900 unidades - Blanco suave</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Fresco Primavera - 900 ml</t>
+          <t>Vais - Limpiador de Frutas - Primavera - 900 ml</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Vais - Jabón Líquido Baja Espuma - Eco Pack - 800 ml</t>
+          <t>Vais - Jabón Líquido Baja Espuma - 800 ml</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Ultra Zombies - Colonia Zombie - 125 ml</t>
+          <t>Ultra Zombies - Colonia 125 - Fragancia intensa - Para hombres y mujeres</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Vais - Limpiador de Baño Gatillo - 500 ml</t>
+          <t>Vais - Limpiador de Baño - Gatillo - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Vais - Baño Refrescante - 900 ml - Azul</t>
+          <t>Vais - Limpiador de Baño - Eco Pack - 900 ml - Sin esfuerzo</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Antigrasa - 900 ml</t>
+          <t>Vais - Limpiador Desengrasante - Eco Pack - 900 ml</t>
         </is>
       </c>
     </row>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Vais - Limpiavidrios Ultra - 900 ml</t>
+          <t>Vais - Limpiavidrios - 900 ml - Transparente - Sin rayas</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Vais - Perfume de Tela Dulces Mimos - 250 ml</t>
+          <t>Vais - Perfumante de Telas Dulces Mimo - 250 ml</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Vais - Perfume Tela Dulces Mimos - 500 ml</t>
+          <t>Vais - Perfumante de Telas Dulces Mimo - 500 ml</t>
         </is>
       </c>
     </row>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Lavanda - 4 - Multiusos</t>
+          <t>Vais - Limpiador de Lavanda - Pack de 4 - Aroma Relajante</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Vais - Limpiador Citrus - 4 - Multiusos - Aroma Cítrico</t>
+          <t>Vais - Limpiador Citrus - Pack de 4 - Refrescante aroma cítrico</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Vais - Repelente Spray - 200 ml - Efecto duradero</t>
+          <t>Vais - Repelente Spray - 200 ml - Insectos - Protección duradera</t>
         </is>
       </c>
     </row>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Vais - Crema Repelente Plus - 200 ml</t>
+          <t>Vais - Repelente Crema Plus - 200 ml</t>
         </is>
       </c>
     </row>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Vais - Repelente Extreme - 200 ml</t>
+          <t>Vais - Repelente Extreme - 200 ml - Transparente - Protección duradera</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Vais - Repelente Kids - Pomo 100 - Sin picaduras</t>
+          <t>Vais - Repelente Infantil - Pomo 100 - Sin Picaduras</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Colonia Mágica - 100 ml</t>
+          <t>Sally Unicornio - Colonia Mágica 100 ml</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Colonia Mágica - 50 ml</t>
+          <t>Sally Unicornio - Colonia 50 ml - Fragancia Floral</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2853,8 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Body Splash - 125 ml</t>
+          <t>Otras características relevantes:
+Sally Unicornio - Fragancia Mágica - 125 ml - Rosa Brillante - Duración prolongada</t>
         </is>
       </c>
     </row>
@@ -2865,7 +2866,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Set Shampoo y Colonia - 200 ml + 125 ml</t>
+          <t>Sally Unicornio - Set de Cabello Brillante - 200 ml + Colonia - 125 ml</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2878,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Espuma de Baño - 350 ml</t>
+          <t>Sally Unicornio - Espuma de Baño - 350 ml - Rosa - Suave y relajante</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2890,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Gel Antibacterial - Soporte 2D - 30 ml</t>
+          <t>Sally Unicornio - Gel Antibacterial - 30 ml - Soporte 2D - Varios colores disponibles</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2902,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Gel Antibacterial Pocket - 60 ml</t>
+          <t>Otras características relevantes: Sally Unicornio - Gel Antibacterial - 60 ml - Transparente - Tamaño de bolsillo</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2914,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Gel Antibacterial Perfumado - 75 ml</t>
+          <t>Sally Unicornio - Gel Antibacterial - 75 ml</t>
         </is>
       </c>
     </row>
@@ -2925,7 +2926,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Sally Unicornio - Acondicionador y Shampoo 2 en 1 - 250 ml</t>
+          <t>Sally Unicornio - Champú y Acondicionador 2 en 1 - 250 ml</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2938,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Ultra Zombies - Set Shampoo + Colonia - 200 ml + 125 ml</t>
+          <t>Ultra Zombies - Combo Zombie Fresh - 2 - Negro - Perfume y afeitadora</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2950,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Algabo Baby - Hisopos de Algodón - Caja 30 unidades</t>
+          <t>Algabo Baby - Caja de hisopos de algodón suave - 30 unidades</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2962,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Hello Kitty - Colonia Dulzura - 125 ml</t>
+          <t>Hello Kitty - Perfume Dulzura - 125 ml</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2986,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Algabo - Talco Clásico - 120 g</t>
+          <t>Algabo - Talco Clásico - 120 gr</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2998,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Algabo - Talco Perfumado Violets - 250 g</t>
+          <t>Algabo - Talco Perfumado - 250 gr - Violets - Fórmula suave y delicada</t>
         </is>
       </c>
     </row>
@@ -3009,7 +3010,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Algabo - Talco Perfumado - 250 g - Floral</t>
+          <t>Algabo - Talco Perfumado Floral - 250 gr</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3022,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Algabo - Spray Refrescante para Pies - 153 ml</t>
+          <t>Algabo - Desodorante refrescante para pies - 153 ml</t>
         </is>
       </c>
     </row>
@@ -3033,7 +3034,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Algabo - Spray Antibacterial para Pies - 200 ml</t>
+          <t>Algabo - Talco Desodorante Antibacterial para pies - 200 gr</t>
         </is>
       </c>
     </row>
@@ -3045,7 +3046,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Algabo - Spray Antibacterial para Pies - 100 ml</t>
+          <t>Algabo - Talco Desodorante Antibacterial para Pies - 100 gr</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3058,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Algabo - Talco Suave - 120 g</t>
+          <t>Algabo - Talco Suave - 120 gr</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3070,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Algabo - Talco Suave - 200 g</t>
+          <t>Algabo - Talco Suave para Pies - 200 gr</t>
         </is>
       </c>
     </row>
@@ -3081,7 +3082,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - 60 ml</t>
+          <t>Algabo - Talco Desodorante para pies - 60 gr</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3094,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Algabo - Talco Suave - 180 g - Rosa</t>
+          <t>Algabo - Talco Suave para pies - 180 gr - Rosa - Fórmula delicada</t>
         </is>
       </c>
     </row>
@@ -3105,7 +3106,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Algabo - Talco Clásico - Eco Pack - 200 g</t>
+          <t>Algabo - Talco clásico - 200g - Blanco</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3118,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies de mujer - 60 ml</t>
+          <t>Algabo - Talco para Pies - 60 gr - Mujer - Fragancia Refrescante</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3130,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - Mujer - 100 ml</t>
+          <t>Algabo - Talco Desodorante para pies mujer - 100 gr.</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3142,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Algabo - Talco Clásico - 180 g</t>
+          <t>Algabo - Talco Suave - 180 gr</t>
         </is>
       </c>
     </row>
@@ -3153,7 +3154,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Algabo - Desodorante Calzado - 153 ml</t>
+          <t>Algabo - Plantillas para calzado - 153 ml</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3166,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Algabo - Talco Perfumado - Bolsita - 200 g</t>
+          <t>Algabo - Talco Perfumado - 200 gr - Bolsita - Aroma suave</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3178,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Algabo - Talco Perfumado - Bolsita - 400 g</t>
+          <t>Algabo - Talco Perfumado - 400 gr - Bolsita</t>
         </is>
       </c>
     </row>
@@ -3201,7 +3202,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Algabo - Fécula Natural - Doypack - 250 ml</t>
+          <t>Algabo - Fécula Natural - 250 g - Transparente - Fácil de usar</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3226,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Algabo - Colonia Inglesa - 500 ml</t>
+          <t>Algabo - Colonia Inglesa - 500 ml - Fragancia Clásica</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3250,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Algabo - Colonia Inglesa - 750 ml</t>
+          <t>Algabo - Colonia Inglesa - 750 ml - Elegante y sofisticada</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3262,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Algabo Kids - Jabón Líquido Suave - 300 ml</t>
+          <t>Algabo Kids - Jabón Suave - 300 ml - Azul - Dermatológicamente probado</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3286,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Manzanilla Mágica - 500 ml</t>
+          <t>Algabo - Jabón Líquido de Manzana y Magnolia - 500 ml</t>
         </is>
       </c>
     </row>
@@ -3309,7 +3310,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Algabo - Jabón Líquido Antibacterial - Doypack - 300 ml</t>
+          <t>Algabo - Jabón Líquido Antibacterial - Doy Pack - 300 ml</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3334,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Algabo - Gel Antibacterial Ultra Pocket - 70 ml</t>
+          <t>Algabo - Gel Sanitizante Ultra Pocket - 70 ml</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3346,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Algabo - Spray Superficies Ultra - 500 ml</t>
+          <t>Algabo - Spray Sanitario Ultra - 500 ml - Superficie - Elimina gérmenes y bacterias</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3358,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Algabo - Espuma Antibacterial Manzana y Magnolia - 250 ml</t>
+          <t>Algabo - Jabón Antibacterial de Manzana y Magnolia - 250 ml</t>
         </is>
       </c>
     </row>
@@ -3369,7 +3370,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - 153 ml</t>
+          <t>Algabo - Desodorante para pies - 153 ml - Blanco - Fórmula refrescante</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3382,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - 200 ml - Hidratante - Suavizante</t>
+          <t>Algabo - Talco Desodorante para pies - 200 gr</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3394,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Hello Kitty - Alegría - 125 ml</t>
+          <t>Hello Kitty - Perfume Alegria - 125 ml - Rosa suave - Fragancia dulce y alegre</t>
         </is>
       </c>
     </row>
@@ -3405,7 +3406,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Avengers - Colonia Hulk - 125 ml</t>
+          <t>Avengers - Colonia Hulk 125 ml - Verde - Fragancia fresca y masculina</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3418,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Spiderman - Sanitizante en Caja - 75 ml</t>
+          <t>Spiderman - Caja Sanitizante - 75 ml</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3430,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Spiderman - Jabón Líquido - Botella 300 ml</t>
+          <t>Spiderman - Jabón líquido - 300 ml - Azul - Suave y refrescante</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3442,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Avengers - Jabón Líquido - Botella 300 ml</t>
+          <t>Avengers - Jabón Líquido Suave - Botella - 300 ml</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3454,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Spiderman - Colonia Superheroica - 125 ml</t>
+          <t>Spiderman - Colonia 125 - Fragancia intensa - Edición especial</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3466,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Avengers - Colonia Capitán América - 125 ml</t>
+          <t>Avengers - Colonia Capitán América 125 ml</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3478,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Avengers - Colonia Iron Man - 125 ml</t>
+          <t>Avengers - Colonia Iron Man 125 ml - Rojo intenso - Fragancia duradera</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3490,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Spiderman - Set de Baño - 125 ml + Shampoo 200 ml</t>
+          <t>Spiderman - Set de cuidado personal - 125 ml + 200 ml - Varios colores disponibles - Ideal para niños</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3502,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - 200 ml</t>
+          <t>Algabo - Talco refrescante para pies - 200 gr</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3526,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Star Wars - Jabón Líquido Baño y Tocador - 300 ml</t>
+          <t>Star Wars - Jabón Líquido Suave - Botella - 300 ml</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3538,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Princesas - Splash Corporal Frozen - 125 ml</t>
+          <t>Princesas - Splash de Cuerpo Congelado - 125 ml - Azul Brillante - Aroma Refrescante</t>
         </is>
       </c>
     </row>
@@ -3549,7 +3550,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Star Wars - Colonia Espacial - 125 ml</t>
+          <t>Star Wars - Colonia Espacial - 125 ml - Azul - Fragancia única y duradera.</t>
         </is>
       </c>
     </row>
@@ -3561,7 +3562,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Princesas - Set Frozen - 125 ml + 200 ml - Azul y Blanco - Edición Especial</t>
+          <t>Princesas - Set de Belleza - 125 ml Colonia + 200 ml Shampoo - Frozen</t>
         </is>
       </c>
     </row>
@@ -3573,7 +3574,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Hello Kitty - Jabón Líquido Botella - 300 ml</t>
+          <t>Hello Kitty - Jabón líquido - Botella 300 ml</t>
         </is>
       </c>
     </row>
@@ -3585,7 +3586,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Spiderman - Soporte Sanitario - 30 unidades</t>
+          <t>Spiderman - Porta Sanitario - 30 unidades</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3598,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Spiderman - Shampoo 200 - Cabello de héroe - Fórmula suave</t>
+          <t>Spiderman - Shampoo Suave - 200 ml</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3610,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Spiderman - Shampoo Spiderman - 350 ml - 2D</t>
+          <t>Spiderman - Shampoo 2 en 1 - 350 ml - Sin enredos - Fórmula suave</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3622,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Spiderman - Autito 2 en 1 - 450 ml</t>
+          <t>Spiderman - Set de baño 2 en 1 - Autito - 450 ml</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3634,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Avengers - Shampoo 2 en 1 - 350 ml - Surtido de personajes</t>
+          <t>Avengers - Shampoo Surtido 350 ml - Pack de 2 - Varios colores</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3646,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Minions - Set Colonia + Shampoo - 125 ml + 200 ml</t>
+          <t>Minions - Set de Fragancia y Shampoo - 125 ml + 200 ml - Fragancia divertida y suave - Ideal para niños</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3658,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Minions - Colonia Fresca - 125 ml</t>
+          <t>Minions - Colonia Fresca 125 ml</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3670,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>GreenWood - Shampoo para Perro y Gato - 500 ml</t>
+          <t>GreenWood - Shampoo para Mascotas - 500 ml - Perro y Gato - Fórmula Suave y Natural</t>
         </is>
       </c>
     </row>
@@ -3681,7 +3682,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Vais - Vestido de Tela Cálida - Primavera - 250 g</t>
+          <t>Vais - Perfumante de Telas Calida Primavera - 250 ml</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3694,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Vais - Perfume Tela - Suave Brisa - 250 ml</t>
+          <t>Vais - Perfume Suave Brisa - 250 ml - Tela</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3706,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Vais - Manta Térmica - Primavera - 500 gramos</t>
+          <t>Vais - Perfume de Telas - Primavera - 500 ml</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3730,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Algabo - Perfume Cálida Primavera - Doypack - 450 ml</t>
+          <t>Algabo - Perfume Cálida y Primaveral - Doble Pack - 450 ml</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3742,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Algabo - Perfume Suave Brisa - Doypack - 450 ml</t>
+          <t>Algabo - Perfume Suave Brisa - Doy Pack - 450 ml</t>
         </is>
       </c>
     </row>
@@ -3753,7 +3754,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Vais - Perfume Suave Brisa - 250 ml</t>
+          <t>Vais - Perfume Brisa Suave - Doy Pack 250 ml - Refrescante</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3766,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Vais - Perfume Cálida Primavera - Doypack - 250 ml</t>
+          <t>Vais - Perfumante de Telas Calida Primavera - 250 ml</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3778,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Algabo - Crema para pies - 100 ml</t>
+          <t>Algabo - Talco Refrescante para Pies - 100 gr</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3790,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>St Valley - Hisopos - Tubo 100 - Blanco - Algodón suave</t>
+          <t>St Valley - Hisopos de Algodón en Tubo - 100 unidades</t>
         </is>
       </c>
     </row>
@@ -3801,7 +3802,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Algabo - Protector Solar Cocoa FPS 50 - Pomo 130 ml</t>
+          <t>Algabo - Protector Solar Cocoa F50 - 130 ml - Sin Parabenos - Resistente al Agua</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3826,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Algabo - Mascarilla Facial Detox - 930 ml</t>
+          <t>Algabo - Acondicionador Refrescante Detox - 930 ml</t>
         </is>
       </c>
     </row>

</xml_diff>